<commit_message>
Module2: TC102 :Added new Automation Test
</commit_message>
<xml_diff>
--- a/TMFramework/DataFiles/Module1.xlsx
+++ b/TMFramework/DataFiles/Module1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
   <si>
     <t>Password</t>
   </si>
@@ -47,6 +47,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -419,18 +420,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="25.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="10.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="10.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="10.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="17.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="15.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="25.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
+    <col min="12" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1">

</xml_diff>